<commit_message>
TetrisGrid.Turn() 함수 BlockType.I 회전 모두 구현
- 공간 없을시 MoveUp() 일단 보류 (기획필요)
</commit_message>
<xml_diff>
--- a/Documents/TetrisGrid_Turn함수설명.xlsx
+++ b/Documents/TetrisGrid_Turn함수설명.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CO4U\GameDev\[Git]Tetris\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cofor\GameDev\[Git]Tetris\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -425,6 +425,18 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -435,18 +447,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -736,7 +736,7 @@
   <dimension ref="A1:R31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W15" sqref="W15"/>
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -746,56 +746,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="23"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="19"/>
     </row>
     <row r="2" spans="1:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="20">
+      <c r="C2" s="16">
         <v>0</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20">
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16">
         <v>1</v>
       </c>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20">
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16">
         <v>2</v>
       </c>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20">
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16">
         <v>3</v>
       </c>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
     </row>
     <row r="3" spans="1:18" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="23" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="2"/>
@@ -816,8 +816,8 @@
       <c r="R3" s="4"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="17"/>
-      <c r="B4" s="19"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="5"/>
       <c r="D4" s="13"/>
       <c r="E4" s="1"/>
@@ -836,8 +836,8 @@
       <c r="R4" s="6"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="17"/>
-      <c r="B5" s="19"/>
+      <c r="A5" s="21"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="5"/>
       <c r="D5" s="11"/>
       <c r="E5" s="1"/>
@@ -856,8 +856,8 @@
       <c r="R5" s="15"/>
     </row>
     <row r="6" spans="1:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="17"/>
-      <c r="B6" s="19"/>
+      <c r="A6" s="21"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="7"/>
       <c r="D6" s="12"/>
       <c r="E6" s="8"/>
@@ -876,21 +876,21 @@
       <c r="R6" s="9"/>
     </row>
     <row r="7" spans="1:18" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="17"/>
-      <c r="B7" s="19" t="s">
+      <c r="A7" s="21"/>
+      <c r="B7" s="23" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="3"/>
+      <c r="D7" s="10"/>
       <c r="E7" s="3"/>
       <c r="F7" s="4"/>
-      <c r="G7" s="2"/>
+      <c r="G7" s="14"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="4"/>
       <c r="K7" s="2"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
       <c r="N7" s="4"/>
       <c r="O7" s="2"/>
       <c r="P7" s="3"/>
@@ -898,30 +898,30 @@
       <c r="R7" s="4"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="17"/>
-      <c r="B8" s="19"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="23"/>
       <c r="C8" s="5"/>
-      <c r="D8" s="1"/>
+      <c r="D8" s="13"/>
       <c r="E8" s="1"/>
       <c r="F8" s="6"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="11"/>
       <c r="J8" s="6"/>
       <c r="K8" s="5"/>
-      <c r="L8" s="1"/>
+      <c r="L8" s="13"/>
       <c r="M8" s="1"/>
       <c r="N8" s="6"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="11"/>
       <c r="R8" s="6"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="17"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="1"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="11"/>
       <c r="E9" s="1"/>
       <c r="F9" s="6"/>
       <c r="G9" s="5"/>
@@ -929,17 +929,17 @@
       <c r="I9" s="1"/>
       <c r="J9" s="6"/>
       <c r="K9" s="5"/>
-      <c r="L9" s="1"/>
+      <c r="L9" s="11"/>
       <c r="M9" s="1"/>
       <c r="N9" s="6"/>
       <c r="O9" s="5"/>
       <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
+      <c r="Q9" s="11"/>
       <c r="R9" s="6"/>
     </row>
     <row r="10" spans="1:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="17"/>
-      <c r="B10" s="19"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="23"/>
       <c r="C10" s="7"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
@@ -958,60 +958,60 @@
       <c r="R10" s="9"/>
     </row>
     <row r="11" spans="1:18" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="17"/>
-      <c r="B11" s="19" t="s">
+      <c r="A11" s="21"/>
+      <c r="B11" s="23" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="3"/>
+      <c r="D11" s="10"/>
       <c r="E11" s="3"/>
       <c r="F11" s="4"/>
       <c r="G11" s="2"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="4"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="3"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
       <c r="M11" s="3"/>
       <c r="N11" s="4"/>
       <c r="O11" s="2"/>
       <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
+      <c r="Q11" s="11"/>
       <c r="R11" s="4"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="17"/>
-      <c r="B12" s="19"/>
+      <c r="A12" s="21"/>
+      <c r="B12" s="23"/>
       <c r="C12" s="5"/>
-      <c r="D12" s="1"/>
+      <c r="D12" s="13"/>
       <c r="E12" s="1"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="11"/>
       <c r="J12" s="6"/>
       <c r="K12" s="5"/>
-      <c r="L12" s="1"/>
+      <c r="L12" s="13"/>
       <c r="M12" s="1"/>
       <c r="N12" s="6"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="11"/>
       <c r="R12" s="6"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="17"/>
-      <c r="B13" s="19"/>
+      <c r="A13" s="21"/>
+      <c r="B13" s="23"/>
       <c r="C13" s="5"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
       <c r="F13" s="6"/>
-      <c r="G13" s="5"/>
+      <c r="G13" s="14"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="6"/>
       <c r="K13" s="5"/>
-      <c r="L13" s="1"/>
+      <c r="L13" s="11"/>
       <c r="M13" s="1"/>
       <c r="N13" s="6"/>
       <c r="O13" s="5"/>
@@ -1020,8 +1020,8 @@
       <c r="R13" s="6"/>
     </row>
     <row r="14" spans="1:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="17"/>
-      <c r="B14" s="19"/>
+      <c r="A14" s="21"/>
+      <c r="B14" s="23"/>
       <c r="C14" s="7"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
@@ -1040,56 +1040,56 @@
       <c r="R14" s="9"/>
     </row>
     <row r="15" spans="1:18" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="17"/>
-      <c r="B15" s="19" t="s">
+      <c r="A15" s="21"/>
+      <c r="B15" s="23" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="4"/>
-      <c r="G15" s="2"/>
+      <c r="G15" s="14"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="4"/>
       <c r="K15" s="2"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
       <c r="N15" s="4"/>
       <c r="O15" s="2"/>
-      <c r="P15" s="3"/>
+      <c r="P15" s="10"/>
       <c r="Q15" s="3"/>
       <c r="R15" s="4"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="17"/>
-      <c r="B16" s="19"/>
+      <c r="A16" s="21"/>
+      <c r="B16" s="23"/>
       <c r="C16" s="5"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="11"/>
       <c r="F16" s="6"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="1"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="13"/>
       <c r="I16" s="1"/>
       <c r="J16" s="6"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="1"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="13"/>
       <c r="M16" s="1"/>
       <c r="N16" s="6"/>
       <c r="O16" s="5"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="11"/>
       <c r="R16" s="6"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="17"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="1"/>
+      <c r="A17" s="21"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="11"/>
       <c r="E17" s="1"/>
       <c r="F17" s="6"/>
       <c r="G17" s="5"/>
-      <c r="H17" s="1"/>
+      <c r="H17" s="11"/>
       <c r="I17" s="1"/>
       <c r="J17" s="6"/>
       <c r="K17" s="5"/>
@@ -1098,12 +1098,12 @@
       <c r="N17" s="6"/>
       <c r="O17" s="5"/>
       <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
+      <c r="Q17" s="11"/>
       <c r="R17" s="6"/>
     </row>
     <row r="18" spans="1:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="17"/>
-      <c r="B18" s="19"/>
+      <c r="A18" s="21"/>
+      <c r="B18" s="23"/>
       <c r="C18" s="7"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
@@ -1122,8 +1122,8 @@
       <c r="R18" s="9"/>
     </row>
     <row r="19" spans="1:18" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="17"/>
-      <c r="B19" s="19" t="s">
+      <c r="A19" s="21"/>
+      <c r="B19" s="23" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="2"/>
@@ -1144,8 +1144,8 @@
       <c r="R19" s="4"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="17"/>
-      <c r="B20" s="19"/>
+      <c r="A20" s="21"/>
+      <c r="B20" s="23"/>
       <c r="C20" s="5"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -1164,8 +1164,8 @@
       <c r="R20" s="6"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A21" s="17"/>
-      <c r="B21" s="19"/>
+      <c r="A21" s="21"/>
+      <c r="B21" s="23"/>
       <c r="C21" s="5"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -1184,8 +1184,8 @@
       <c r="R21" s="6"/>
     </row>
     <row r="22" spans="1:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="17"/>
-      <c r="B22" s="19"/>
+      <c r="A22" s="21"/>
+      <c r="B22" s="23"/>
       <c r="C22" s="7"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
@@ -1204,8 +1204,8 @@
       <c r="R22" s="9"/>
     </row>
     <row r="23" spans="1:18" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="17"/>
-      <c r="B23" s="19" t="s">
+      <c r="A23" s="21"/>
+      <c r="B23" s="23" t="s">
         <v>6</v>
       </c>
       <c r="C23" s="2"/>
@@ -1226,8 +1226,8 @@
       <c r="R23" s="4"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A24" s="17"/>
-      <c r="B24" s="19"/>
+      <c r="A24" s="21"/>
+      <c r="B24" s="23"/>
       <c r="C24" s="5"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -1246,8 +1246,8 @@
       <c r="R24" s="6"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A25" s="17"/>
-      <c r="B25" s="19"/>
+      <c r="A25" s="21"/>
+      <c r="B25" s="23"/>
       <c r="C25" s="5"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -1266,8 +1266,8 @@
       <c r="R25" s="6"/>
     </row>
     <row r="26" spans="1:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="17"/>
-      <c r="B26" s="19"/>
+      <c r="A26" s="21"/>
+      <c r="B26" s="23"/>
       <c r="C26" s="7"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
@@ -1286,8 +1286,8 @@
       <c r="R26" s="9"/>
     </row>
     <row r="27" spans="1:18" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="17"/>
-      <c r="B27" s="19" t="s">
+      <c r="A27" s="21"/>
+      <c r="B27" s="23" t="s">
         <v>7</v>
       </c>
       <c r="C27" s="2"/>
@@ -1308,8 +1308,8 @@
       <c r="R27" s="4"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A28" s="17"/>
-      <c r="B28" s="19"/>
+      <c r="A28" s="21"/>
+      <c r="B28" s="23"/>
       <c r="C28" s="5"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -1328,8 +1328,8 @@
       <c r="R28" s="6"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A29" s="17"/>
-      <c r="B29" s="19"/>
+      <c r="A29" s="21"/>
+      <c r="B29" s="23"/>
       <c r="C29" s="5"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -1348,8 +1348,8 @@
       <c r="R29" s="6"/>
     </row>
     <row r="30" spans="1:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="18"/>
-      <c r="B30" s="19"/>
+      <c r="A30" s="22"/>
+      <c r="B30" s="23"/>
       <c r="C30" s="7"/>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
@@ -1370,11 +1370,6 @@
     <row r="31" spans="1:18" ht="17.25" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="C1:R1"/>
     <mergeCell ref="A3:A30"/>
     <mergeCell ref="B7:B10"/>
     <mergeCell ref="B11:B14"/>
@@ -1383,6 +1378,11 @@
     <mergeCell ref="B23:B26"/>
     <mergeCell ref="B27:B30"/>
     <mergeCell ref="B3:B6"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="C1:R1"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
TetrisGrid.Turn() 구현 완료, GameManager,GeneratePlayerGrid() 코딩 시작
</commit_message>
<xml_diff>
--- a/Documents/TetrisGrid_Turn함수설명.xlsx
+++ b/Documents/TetrisGrid_Turn함수설명.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>_blockTurnState</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -127,6 +127,22 @@
   </si>
   <si>
     <t>위</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>위</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>오</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>아</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>왼</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -803,8 +819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1315,59 +1331,67 @@
         <v>6</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="D23" s="3"/>
+      <c r="D23" s="2"/>
       <c r="E23" s="3"/>
       <c r="F23" s="4"/>
       <c r="G23" s="1"/>
-      <c r="H23" s="3"/>
+      <c r="H23" s="2"/>
       <c r="I23" s="3"/>
       <c r="J23" s="4"/>
       <c r="K23" s="1"/>
-      <c r="L23" s="3"/>
+      <c r="L23" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="M23" s="3"/>
       <c r="N23" s="4"/>
       <c r="O23" s="1"/>
-      <c r="P23" s="3"/>
+      <c r="P23" s="2"/>
       <c r="Q23" s="3"/>
       <c r="R23" s="4"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="21"/>
       <c r="B24" s="23"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="10"/>
       <c r="F24" s="8"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
+      <c r="G24" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H24" s="6"/>
+      <c r="I24" s="10"/>
       <c r="J24" s="8"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="10"/>
       <c r="N24" s="8"/>
-      <c r="O24" s="5"/>
-      <c r="P24" s="7"/>
-      <c r="Q24" s="7"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="7" t="s">
+        <v>29</v>
+      </c>
       <c r="R24" s="8"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="21"/>
       <c r="B25" s="23"/>
       <c r="C25" s="5"/>
-      <c r="D25" s="7"/>
+      <c r="D25" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="E25" s="7"/>
       <c r="F25" s="8"/>
       <c r="G25" s="5"/>
-      <c r="H25" s="7"/>
+      <c r="H25" s="10"/>
       <c r="I25" s="7"/>
       <c r="J25" s="8"/>
       <c r="K25" s="5"/>
-      <c r="L25" s="7"/>
+      <c r="L25" s="10"/>
       <c r="M25" s="7"/>
       <c r="N25" s="8"/>
       <c r="O25" s="5"/>
-      <c r="P25" s="7"/>
+      <c r="P25" s="10"/>
       <c r="Q25" s="7"/>
       <c r="R25" s="8"/>
     </row>
@@ -1396,8 +1420,8 @@
       <c r="B27" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="3"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="2"/>
       <c r="E27" s="3"/>
       <c r="F27" s="4"/>
       <c r="G27" s="1"/>
@@ -1416,8 +1440,8 @@
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="21"/>
       <c r="B28" s="23"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="7"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="10"/>
       <c r="E28" s="7"/>
       <c r="F28" s="8"/>
       <c r="G28" s="5"/>

</xml_diff>